<commit_message>
script logic and input csvs
</commit_message>
<xml_diff>
--- a/input files/su25/M3 wavelengths targeted global.xlsx
+++ b/input files/su25/M3 wavelengths targeted global.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janicebishop/Documents/Janice_files/Research/Moon/LDAP_M3_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Documents/Productivity/SETI/m3-lunar-project/input files/su25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210E7743-2464-1846-9239-D13B01706EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5233B7-6E0F-9D44-9F63-D68F242D94D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="1560" windowWidth="31440" windowHeight="20840" xr2:uid="{4C69846C-142E-2C4F-A090-E7CDB9AB41B1}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{4C69846C-142E-2C4F-A090-E7CDB9AB41B1}"/>
   </bookViews>
   <sheets>
     <sheet name="M3-global-wavelengths" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Wavelength (µm) M3 targeted images</t>
   </si>
@@ -61,6 +61,12 @@
   <si>
     <t>average every 4 channels, step n, sort, round 0.0001</t>
   </si>
+  <si>
+    <t>should stay step 4</t>
+  </si>
+  <si>
+    <t>move values up (1.6587 here)</t>
+  </si>
 </sst>
 </file>
 
@@ -73,21 +79,21 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Aptos Display"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -95,7 +101,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -103,7 +109,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -111,35 +117,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -147,7 +153,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -155,14 +161,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -170,14 +176,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -185,7 +191,7 @@
       <i/>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -193,14 +199,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -618,39 +624,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -702,7 +708,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -813,6 +819,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -821,13 +834,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -892,31 +898,11 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -926,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360BED3D-739B-264D-8715-7DE683017645}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146:A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2572,6 +2558,12 @@
       <c r="A122">
         <v>1.6436999999999999</v>
       </c>
+      <c r="C122" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">

</xml_diff>